<commit_message>
Final changes of 20th May 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_PrePROD.xlsx
+++ b/RTE/src/main/resources/RTE_PrePROD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
@@ -29,18 +29,6 @@
     <t>RWTrackingNo</t>
   </si>
   <si>
-    <t>RTE Job Creation</t>
-  </si>
-  <si>
-    <t>RT00002183</t>
-  </si>
-  <si>
-    <t>RTE Job Creation ForCrud</t>
-  </si>
-  <si>
-    <t>RT00002194</t>
-  </si>
-  <si>
     <t>JobID</t>
   </si>
   <si>
@@ -231,6 +219,18 @@
   </si>
   <si>
     <t>126040067</t>
+  </si>
+  <si>
+    <t>RT00001880</t>
+  </si>
+  <si>
+    <t>RTE Job Creation_PreProd</t>
+  </si>
+  <si>
+    <t>RTE Job Creation ForCrud_PreProd</t>
+  </si>
+  <si>
+    <t>RT00001881</t>
   </si>
 </sst>
 </file>
@@ -1124,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,24 +1148,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1192,41 +1192,41 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
         <v>64</v>
       </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1262,76 +1262,76 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="I1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="L1" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
       <c r="K2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="M2" s="2"/>
     </row>
@@ -1485,100 +1485,100 @@
         <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>39</v>
-      </c>
       <c r="K1" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
         <v>47</v>
       </c>
-      <c r="E2" t="s">
+      <c r="K2" t="s">
         <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
         <v>53</v>
       </c>
-      <c r="D3" t="s">
+      <c r="I3" t="s">
         <v>54</v>
       </c>
-      <c r="E3" t="s">
+      <c r="J3" t="s">
         <v>55</v>
       </c>
-      <c r="F3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" t="s">
-        <v>59</v>
-      </c>
       <c r="K3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1694,7 +1694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -1709,42 +1709,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fiinal changes of 26th May 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE_PrePROD.xlsx
+++ b/RTE/src/main/resources/RTE_PrePROD.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="17235" windowHeight="7755"/>
+    <workbookView windowHeight="7755" windowWidth="17235" xWindow="120" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="RTECreation" sheetId="1" r:id="rId1"/>
-    <sheet name="SearchRTE" sheetId="2" r:id="rId2"/>
-    <sheet name="Rate" sheetId="3" r:id="rId3"/>
-    <sheet name="RouteDetail" sheetId="4" r:id="rId4"/>
-    <sheet name="ShipmentDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="RTECreation" r:id="rId1" sheetId="1"/>
+    <sheet name="SearchRTE" r:id="rId2" sheetId="2"/>
+    <sheet name="Rate" r:id="rId3" sheetId="3"/>
+    <sheet name="RouteDetail" r:id="rId4" sheetId="4"/>
+    <sheet name="ShipmentDetails" r:id="rId5" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
   <si>
     <t>FileName</t>
   </si>
@@ -231,12 +231,64 @@
   </si>
   <si>
     <t>RT00001881</t>
+  </si>
+  <si>
+    <t>One To One</t>
+  </si>
+  <si>
+    <t>One To Many</t>
+  </si>
+  <si>
+    <t>Many to One</t>
+  </si>
+  <si>
+    <t>Many To Many</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>RTE Job Creation OneToMany_PreProd</t>
+  </si>
+  <si>
+    <t>RTE Job Creation ManyToOne_PreProd</t>
+  </si>
+  <si>
+    <t>RTE Job Creation ManyToMany_PreProd</t>
+  </si>
+  <si>
+    <t>RTE Job Creation Manual__PreProd</t>
+  </si>
+  <si>
+    <t>RT00001882</t>
+  </si>
+  <si>
+    <t>RT00001883</t>
+  </si>
+  <si>
+    <t>RT00001884</t>
+  </si>
+  <si>
+    <t>RT00001885</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>32255478</t>
+  </si>
+  <si>
+    <t>3260720</t>
+  </si>
+  <si>
+    <t>320017960635</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -651,114 +703,117 @@
     </border>
   </borders>
   <cellStyleXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="20" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="6" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="21" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="5" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="7" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="10" fontId="8" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="8" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="9" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="13" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="14" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="15" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="16" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="17" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="22" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="18" fontId="9" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="3" fontId="10" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="11" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="23" fontId="12" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="13" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="4" fontId="14" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="4" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="5" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="6" fontId="15" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="6" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="24" fontId="16" numFmtId="0"/>
+    <xf applyAlignment="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="9" fillId="25" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyNumberFormat="0" applyProtection="0" borderId="10" fillId="6" fontId="17" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="18" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="19" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="10">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="19" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="26" fontId="18" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="26" fontId="18" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
+    <cellStyle builtinId="30" customBuiltin="1" name="20% - Accent1" xfId="1"/>
+    <cellStyle builtinId="34" customBuiltin="1" name="20% - Accent2" xfId="2"/>
+    <cellStyle builtinId="38" customBuiltin="1" name="20% - Accent3" xfId="3"/>
+    <cellStyle builtinId="42" customBuiltin="1" name="20% - Accent4" xfId="4"/>
+    <cellStyle builtinId="46" customBuiltin="1" name="20% - Accent5" xfId="5"/>
+    <cellStyle builtinId="50" customBuiltin="1" name="20% - Accent6" xfId="6"/>
+    <cellStyle builtinId="31" customBuiltin="1" name="40% - Accent1" xfId="7"/>
+    <cellStyle builtinId="35" customBuiltin="1" name="40% - Accent2" xfId="8"/>
+    <cellStyle builtinId="39" customBuiltin="1" name="40% - Accent3" xfId="9"/>
+    <cellStyle builtinId="43" customBuiltin="1" name="40% - Accent4" xfId="10"/>
+    <cellStyle builtinId="47" customBuiltin="1" name="40% - Accent5" xfId="11"/>
+    <cellStyle builtinId="51" customBuiltin="1" name="40% - Accent6" xfId="12"/>
+    <cellStyle builtinId="32" customBuiltin="1" name="60% - Accent1" xfId="13"/>
+    <cellStyle builtinId="36" customBuiltin="1" name="60% - Accent2" xfId="14"/>
+    <cellStyle builtinId="40" customBuiltin="1" name="60% - Accent3" xfId="15"/>
+    <cellStyle builtinId="44" customBuiltin="1" name="60% - Accent4" xfId="16"/>
+    <cellStyle builtinId="48" customBuiltin="1" name="60% - Accent5" xfId="17"/>
+    <cellStyle builtinId="52" customBuiltin="1" name="60% - Accent6" xfId="18"/>
+    <cellStyle builtinId="29" customBuiltin="1" name="Accent1" xfId="19"/>
+    <cellStyle builtinId="33" customBuiltin="1" name="Accent2" xfId="20"/>
+    <cellStyle builtinId="37" customBuiltin="1" name="Accent3" xfId="21"/>
+    <cellStyle builtinId="41" customBuiltin="1" name="Accent4" xfId="22"/>
+    <cellStyle builtinId="45" customBuiltin="1" name="Accent5" xfId="23"/>
+    <cellStyle builtinId="49" customBuiltin="1" name="Accent6" xfId="24"/>
+    <cellStyle builtinId="27" customBuiltin="1" name="Bad" xfId="25"/>
+    <cellStyle builtinId="22" customBuiltin="1" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="23" customBuiltin="1" name="Check Cell" xfId="27"/>
+    <cellStyle builtinId="53" customBuiltin="1" name="Explanatory Text" xfId="28"/>
+    <cellStyle builtinId="26" customBuiltin="1" name="Good" xfId="29"/>
+    <cellStyle builtinId="16" customBuiltin="1" name="Heading 1" xfId="30"/>
+    <cellStyle builtinId="17" customBuiltin="1" name="Heading 2" xfId="31"/>
+    <cellStyle builtinId="18" customBuiltin="1" name="Heading 3" xfId="32"/>
+    <cellStyle builtinId="19" customBuiltin="1" name="Heading 4" xfId="33"/>
+    <cellStyle builtinId="20" customBuiltin="1" name="Input" xfId="34"/>
+    <cellStyle builtinId="24" customBuiltin="1" name="Linked Cell" xfId="35"/>
+    <cellStyle builtinId="28" customBuiltin="1" name="Neutral" xfId="36"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="10" customBuiltin="1" name="Note" xfId="37"/>
+    <cellStyle builtinId="21" customBuiltin="1" name="Output" xfId="38"/>
+    <cellStyle builtinId="15" customBuiltin="1" name="Title" xfId="39"/>
+    <cellStyle builtinId="25" customBuiltin="1" name="Total" xfId="40"/>
+    <cellStyle builtinId="11" customBuiltin="1" name="Warning Text" xfId="41"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -840,10 +895,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1001,7 +1056,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1010,13 +1065,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1026,7 +1081,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1035,7 +1090,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1044,7 +1099,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1054,12 +1109,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1090,7 +1145,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1109,7 +1164,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1121,21 +1176,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="40.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1145,8 +1201,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
@@ -1154,10 +1213,13 @@
         <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -1165,26 +1227,84 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>84</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="9" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1203,42 +1323,72 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>66</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1246,15 +1396,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1456,14 +1606,14 @@
       <c r="M10" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
@@ -1471,16 +1621,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1515,7 +1665,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row ht="60" r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -1550,7 +1700,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row ht="60" r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="8"/>
       <c r="C3" t="s">
@@ -1686,13 +1836,13 @@
       <c r="K11" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
@@ -1700,11 +1850,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1820,6 +1970,6 @@
       <c r="F11" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>